<commit_message>
Actualizacion de archivo de autocorreccion
</commit_message>
<xml_diff>
--- a/correcciones20162C.xlsx
+++ b/correcciones20162C.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Tp-PW3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="148">
   <si>
     <t xml:space="preserve">Página de inicio​ (​/default.aspx​)  </t>
   </si>
@@ -794,6 +794,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -801,15 +810,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2480,10 +2480,10 @@
   <dimension ref="A1:O181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F177" sqref="F177:F181"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,14 +2530,14 @@
       </c>
       <c r="K1">
         <f>COUNTIF(F:F, "B")</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>146</v>
       </c>
       <c r="M1" s="14">
         <f>K1/I1</f>
-        <v>0</v>
+        <v>0.32374100719424459</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>137</v>
@@ -2551,15 +2551,15 @@
       <c r="A2" s="11">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -2571,6 +2571,9 @@
       <c r="E3" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F3" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -2582,6 +2585,9 @@
       <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F4" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
@@ -2593,31 +2599,33 @@
       <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="9"/>
+      <c r="F5" s="9" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>1</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="17"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="20"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2626,6 +2634,9 @@
       </c>
       <c r="E8" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -2637,6 +2648,9 @@
       <c r="E9" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F9" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
@@ -2655,6 +2669,9 @@
       <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F11" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D12" s="5" t="s">
@@ -2663,15 +2680,18 @@
       <c r="E12" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F12" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
@@ -2683,12 +2703,12 @@
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" s="5" t="s">
@@ -2742,13 +2762,13 @@
       <c r="A22" s="11">
         <v>2</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="20"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
@@ -2757,6 +2777,9 @@
       <c r="E23" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F23" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="5" t="s">
@@ -2765,6 +2788,9 @@
       <c r="E24" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F24" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D25" s="5" t="s">
@@ -2773,6 +2799,9 @@
       <c r="E25" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F25" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D26" s="5" t="s">
@@ -2781,6 +2810,9 @@
       <c r="E26" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F26" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D27" s="5" t="s">
@@ -2789,6 +2821,9 @@
       <c r="E27" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F27" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D28" s="5" t="s">
@@ -2797,6 +2832,9 @@
       <c r="E28" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F28" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D29" s="5" t="s">
@@ -2805,13 +2843,16 @@
       <c r="E29" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F29" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="17"/>
+      <c r="D30" s="20"/>
     </row>
     <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D31" s="9" t="s">
@@ -2833,13 +2874,13 @@
       <c r="A33" s="11">
         <v>3</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="20"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="17"/>
     </row>
     <row r="34" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D34" s="4" t="s">
@@ -2847,6 +2888,9 @@
       </c>
       <c r="E34" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2858,6 +2902,9 @@
       <c r="E35" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F35" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
@@ -2876,6 +2923,9 @@
       <c r="E37" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F37" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D38" s="5" t="s">
@@ -2884,15 +2934,18 @@
       <c r="E38" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F38" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="17"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="20"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
@@ -2972,12 +3025,12 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="17"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="20"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
@@ -3011,15 +3064,15 @@
       <c r="A52" s="11">
         <v>4</v>
       </c>
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19" t="s">
+      <c r="C52" s="16"/>
+      <c r="D52" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E52" s="19"/>
-      <c r="F52" s="20"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="17"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D53" s="4" t="s">
@@ -3027,6 +3080,9 @@
       </c>
       <c r="E53" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3038,6 +3094,9 @@
       <c r="E54" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F54" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
@@ -3056,14 +3115,17 @@
       <c r="E56" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F56" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="17"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="20"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D58" s="5" t="s">
@@ -3098,12 +3160,12 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="17"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="20"/>
     </row>
     <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D63" s="5" t="s">
@@ -3117,15 +3179,15 @@
       <c r="A64" s="11">
         <v>5</v>
       </c>
-      <c r="B64" s="18" t="s">
+      <c r="B64" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D64" s="19"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="20"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="17"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D65" s="4" t="s">
@@ -3133,6 +3195,9 @@
       </c>
       <c r="E65" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3144,6 +3209,9 @@
       <c r="E66" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F66" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
@@ -3162,14 +3230,17 @@
       <c r="E68" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F68" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C69" s="15" t="s">
+      <c r="C69" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="16"/>
-      <c r="E69" s="16"/>
-      <c r="F69" s="17"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="20"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D70" s="5" t="s">
@@ -3364,12 +3435,12 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C94" s="15" t="s">
+      <c r="C94" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D94" s="16"/>
-      <c r="E94" s="16"/>
-      <c r="F94" s="17"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="20"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D95" s="5" t="s">
@@ -3383,15 +3454,15 @@
       <c r="A96" s="11">
         <v>6</v>
       </c>
-      <c r="B96" s="18" t="s">
+      <c r="B96" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C96" s="19" t="s">
+      <c r="C96" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D96" s="19"/>
-      <c r="E96" s="19"/>
-      <c r="F96" s="20"/>
+      <c r="D96" s="16"/>
+      <c r="E96" s="16"/>
+      <c r="F96" s="17"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D97" s="4" t="s">
@@ -3399,6 +3470,9 @@
       </c>
       <c r="E97" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3410,6 +3484,9 @@
       <c r="E98" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F98" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B99" s="6"/>
@@ -3428,14 +3505,17 @@
       <c r="E100" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F100" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C101" s="15" t="s">
+      <c r="C101" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D101" s="16"/>
-      <c r="E101" s="16"/>
-      <c r="F101" s="17"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="20"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D102" s="5" t="s">
@@ -3488,12 +3568,12 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C108" s="15" t="s">
+      <c r="C108" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D108" s="16"/>
-      <c r="E108" s="16"/>
-      <c r="F108" s="17"/>
+      <c r="D108" s="19"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="20"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D109" s="5" t="s">
@@ -3507,15 +3587,15 @@
       <c r="A110" s="11">
         <v>7</v>
       </c>
-      <c r="B110" s="18" t="s">
+      <c r="B110" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C110" s="19" t="s">
+      <c r="C110" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="D110" s="19"/>
-      <c r="E110" s="19"/>
-      <c r="F110" s="20"/>
+      <c r="D110" s="16"/>
+      <c r="E110" s="16"/>
+      <c r="F110" s="17"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D111" s="4" t="s">
@@ -3523,6 +3603,9 @@
       </c>
       <c r="E111" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3534,6 +3617,9 @@
       <c r="E112" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F112" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B113" s="6"/>
@@ -3552,6 +3638,9 @@
       <c r="E114" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F114" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D115" s="5" t="s">
@@ -3560,14 +3649,17 @@
       <c r="E115" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F115" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C116" s="15" t="s">
+      <c r="C116" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="16"/>
-      <c r="E116" s="16"/>
-      <c r="F116" s="17"/>
+      <c r="D116" s="19"/>
+      <c r="E116" s="19"/>
+      <c r="F116" s="20"/>
     </row>
     <row r="117" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="7"/>
@@ -3596,12 +3688,12 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C120" s="15" t="s">
+      <c r="C120" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D120" s="16"/>
-      <c r="E120" s="16"/>
-      <c r="F120" s="17"/>
+      <c r="D120" s="19"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="20"/>
     </row>
     <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D121" s="5" t="s">
@@ -3615,15 +3707,15 @@
       <c r="A122" s="11">
         <v>8</v>
       </c>
-      <c r="B122" s="18" t="s">
+      <c r="B122" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C122" s="19" t="s">
+      <c r="C122" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D122" s="19"/>
-      <c r="E122" s="19"/>
-      <c r="F122" s="20"/>
+      <c r="D122" s="16"/>
+      <c r="E122" s="16"/>
+      <c r="F122" s="17"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D123" s="4" t="s">
@@ -3631,6 +3723,9 @@
       </c>
       <c r="E123" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3642,6 +3737,9 @@
       <c r="E124" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F124" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B125" s="6"/>
@@ -3660,6 +3758,9 @@
       <c r="E126" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F126" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D127" s="5" t="s">
@@ -3670,12 +3771,12 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C128" s="15" t="s">
+      <c r="C128" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D128" s="16"/>
-      <c r="E128" s="16"/>
-      <c r="F128" s="17"/>
+      <c r="D128" s="19"/>
+      <c r="E128" s="19"/>
+      <c r="F128" s="20"/>
     </row>
     <row r="129" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C129" s="7"/>
@@ -3690,15 +3791,15 @@
       <c r="A130" s="11">
         <v>8.1</v>
       </c>
-      <c r="B130" s="18" t="s">
+      <c r="B130" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C130" s="19" t="s">
+      <c r="C130" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D130" s="19"/>
-      <c r="E130" s="19"/>
-      <c r="F130" s="20"/>
+      <c r="D130" s="16"/>
+      <c r="E130" s="16"/>
+      <c r="F130" s="17"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D131" s="4" t="s">
@@ -3706,6 +3807,9 @@
       </c>
       <c r="E131" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="F131" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3717,6 +3821,9 @@
       <c r="E132" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F132" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
@@ -3735,6 +3842,9 @@
       <c r="E134" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F134" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D135" s="5" t="s">
@@ -3809,12 +3919,12 @@
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C144" s="15" t="s">
+      <c r="C144" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D144" s="16"/>
-      <c r="E144" s="16"/>
-      <c r="F144" s="17"/>
+      <c r="D144" s="19"/>
+      <c r="E144" s="19"/>
+      <c r="F144" s="20"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D145" s="5" t="s">
@@ -3889,12 +3999,12 @@
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C154" s="15" t="s">
+      <c r="C154" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D154" s="16"/>
-      <c r="E154" s="16"/>
-      <c r="F154" s="17"/>
+      <c r="D154" s="19"/>
+      <c r="E154" s="19"/>
+      <c r="F154" s="20"/>
     </row>
     <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D155" s="5" t="s">
@@ -3916,15 +4026,15 @@
       <c r="A157" s="11">
         <v>9</v>
       </c>
-      <c r="B157" s="18" t="s">
+      <c r="B157" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C157" s="19" t="s">
+      <c r="C157" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="D157" s="19"/>
-      <c r="E157" s="19"/>
-      <c r="F157" s="20"/>
+      <c r="D157" s="16"/>
+      <c r="E157" s="16"/>
+      <c r="F157" s="17"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D158" s="4" t="s">
@@ -3932,6 +4042,9 @@
       </c>
       <c r="E158" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="F158" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3943,6 +4056,9 @@
       <c r="E159" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F159" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
@@ -3961,6 +4077,9 @@
       <c r="E161" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F161" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D162" s="5" t="s">
@@ -4006,15 +4125,15 @@
       <c r="A167" s="11">
         <v>10</v>
       </c>
-      <c r="B167" s="18" t="s">
+      <c r="B167" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C167" s="19" t="s">
+      <c r="C167" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D167" s="19"/>
-      <c r="E167" s="19"/>
-      <c r="F167" s="20"/>
+      <c r="D167" s="16"/>
+      <c r="E167" s="16"/>
+      <c r="F167" s="17"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D168" s="4" t="s">
@@ -4088,58 +4207,87 @@
       <c r="A176" s="11">
         <v>11</v>
       </c>
-      <c r="B176" s="18" t="s">
+      <c r="B176" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C176" s="19" t="s">
+      <c r="C176" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="D176" s="19"/>
-      <c r="E176" s="19"/>
-      <c r="F176" s="20"/>
-    </row>
-    <row r="177" spans="4:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D176" s="16"/>
+      <c r="E176" s="16"/>
+      <c r="F176" s="17"/>
+    </row>
+    <row r="177" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D177" s="5" t="s">
         <v>120</v>
       </c>
       <c r="E177" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="178" spans="4:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F177" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="178" spans="4:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D178" s="5" t="s">
         <v>121</v>
       </c>
       <c r="E178" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="179" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F178" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="179" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D179" s="5" t="s">
         <v>122</v>
       </c>
       <c r="E179" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="180" spans="4:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F179" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="180" spans="4:6" ht="75" x14ac:dyDescent="0.25">
       <c r="D180" s="5" t="s">
         <v>123</v>
       </c>
       <c r="E180" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="181" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F180" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="181" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D181" s="5" t="s">
         <v>147</v>
       </c>
       <c r="E181" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F181" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C154:F154"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="C108:F108"/>
+    <mergeCell ref="C116:F116"/>
+    <mergeCell ref="C120:F120"/>
+    <mergeCell ref="C128:F128"/>
+    <mergeCell ref="C144:F144"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B22:F22"/>
@@ -4156,20 +4304,6 @@
     <mergeCell ref="C39:F39"/>
     <mergeCell ref="C48:F48"/>
     <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C154:F154"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C69:F69"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="C108:F108"/>
-    <mergeCell ref="C116:F116"/>
-    <mergeCell ref="C120:F120"/>
-    <mergeCell ref="C128:F128"/>
-    <mergeCell ref="C144:F144"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E21 E149:E153 E1 E11:E12 E37:E38 E56 E100 E161:E166 E171:E175 E14 E23:E32 E40:E47 E63 E49:E51 E58:E61 E68 E81:E93 E70:E78 E102:E107 E117:E119 E121 E129 E95 E109 E114:E115 E134:E143 E155:E156 E3:E5 E126:E127 E177:E1048576">
     <cfRule type="cellIs" dxfId="134" priority="140" operator="equal">

</xml_diff>